<commit_message>
Finalization of endpoint documentation
</commit_message>
<xml_diff>
--- a/documentation/planning/planning_previsionnel_travail_de_diplome .xlsx
+++ b/documentation/planning/planning_previsionnel_travail_de_diplome .xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\bj-travail-diplome-2021\documentation\planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C570A6F7-B48A-4D8F-B9C6-6714EF2C615C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF90AE63-6B4E-4F81-9CFE-4BC082D17ED2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1230" yWindow="2385" windowWidth="23700" windowHeight="13365" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planning" sheetId="1" r:id="rId1"/>
@@ -224,50 +224,50 @@
 par jour :</t>
   </si>
   <si>
-    <t>Duére d'une
+    <t>API Rest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">API routes </t>
+  </si>
+  <si>
+    <t>Appoitment</t>
+  </si>
+  <si>
+    <t>Planning</t>
+  </si>
+  <si>
+    <t>Absence</t>
+  </si>
+  <si>
+    <t>Onglet rendez-vous autonome</t>
+  </si>
+  <si>
+    <t>Connexion</t>
+  </si>
+  <si>
+    <t>Progressive web app</t>
+  </si>
+  <si>
+    <t>Onglet d'affichage de tous les clients</t>
+  </si>
+  <si>
+    <t>Onglet des contenus séances d'un client</t>
+  </si>
+  <si>
+    <t>Onglet d'ajout de documents</t>
+  </si>
+  <si>
+    <t>Gestion des disponiblités de l'éducateur canin</t>
+  </si>
+  <si>
+    <t>Onglet de validation de fiche client</t>
+  </si>
+  <si>
+    <t>Onglet contenus séances</t>
+  </si>
+  <si>
+    <t>Durée d'une
  période :</t>
-  </si>
-  <si>
-    <t>API Rest</t>
-  </si>
-  <si>
-    <t xml:space="preserve">API routes </t>
-  </si>
-  <si>
-    <t>Appoitment</t>
-  </si>
-  <si>
-    <t>Planning</t>
-  </si>
-  <si>
-    <t>Absence</t>
-  </si>
-  <si>
-    <t>Onglet rendez-vous autonome</t>
-  </si>
-  <si>
-    <t>Connexion</t>
-  </si>
-  <si>
-    <t>Progressive web app</t>
-  </si>
-  <si>
-    <t>Onglet d'affichage de tous les clients</t>
-  </si>
-  <si>
-    <t>Onglet des contenus séances d'un client</t>
-  </si>
-  <si>
-    <t>Onglet d'ajout de documents</t>
-  </si>
-  <si>
-    <t>Gestion des disponiblités de l'éducateur canin</t>
-  </si>
-  <si>
-    <t>Onglet de validation de fiche client</t>
-  </si>
-  <si>
-    <t>Onglet contenus séances</t>
   </si>
 </sst>
 </file>
@@ -1107,8 +1107,8 @@
   </sheetPr>
   <dimension ref="A1:BT39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="U1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AR6" sqref="AR6:AR7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1401,7 +1401,7 @@
     </row>
     <row r="3" spans="1:72" s="16" customFormat="1" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="35" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B3" s="36"/>
       <c r="C3" s="37"/>
@@ -1457,7 +1457,7 @@
     </row>
     <row r="4" spans="1:72" s="40" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="43" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B4" s="41"/>
       <c r="C4" s="64"/>
@@ -1502,7 +1502,7 @@
       <c r="AP4" s="63"/>
       <c r="AQ4" s="41"/>
       <c r="AR4" s="72" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="AS4" s="68">
         <v>3.125E-2</v>
@@ -1715,7 +1715,7 @@
     </row>
     <row r="8" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B8" s="18">
         <v>8</v>
@@ -1773,7 +1773,7 @@
     </row>
     <row r="9" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B9" s="18">
         <v>16</v>
@@ -1835,7 +1835,7 @@
     </row>
     <row r="10" spans="1:72" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B10" s="18">
         <v>4</v>
@@ -2043,7 +2043,7 @@
     </row>
     <row r="13" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B13" s="20">
         <v>4</v>
@@ -2215,7 +2215,7 @@
     </row>
     <row r="16" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B16" s="20">
         <v>8</v>
@@ -2349,7 +2349,7 @@
     </row>
     <row r="18" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B18" s="20">
         <v>4</v>
@@ -2575,7 +2575,7 @@
     </row>
     <row r="22" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B22" s="20">
         <v>4</v>
@@ -2633,7 +2633,7 @@
     </row>
     <row r="23" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B23" s="20">
         <v>4</v>
@@ -2689,7 +2689,7 @@
     </row>
     <row r="24" spans="1:72" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B24" s="20">
         <v>4</v>
@@ -2821,7 +2821,7 @@
     </row>
     <row r="26" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B26" s="20">
         <v>8</v>
@@ -2935,7 +2935,7 @@
     </row>
     <row r="28" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B28" s="20">
         <v>6</v>
@@ -3049,7 +3049,7 @@
     </row>
     <row r="30" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B30" s="20">
         <v>16</v>

</xml_diff>